<commit_message>
Adding SEM, scatter plots into graphs
</commit_message>
<xml_diff>
--- a/young-DSS-exp2/new_weight_measurement.xlsx
+++ b/young-DSS-exp2/new_weight_measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\young-DSS-exp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963696DC-5CB9-4669-9588-BA73E410D791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854A707-F05E-4EC9-A89F-4C92846F8601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{B39F8DC0-D618-4399-8ED4-92D19BDDA9D8}"/>
   </bookViews>
@@ -440,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9694913F-0376-40DD-B748-937DACB00989}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +464,14 @@
       <c r="E1" s="1">
         <v>45357</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F1" s="1">
+        <v>45364</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -481,8 +487,14 @@
       <c r="E2">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F2" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -498,8 +510,14 @@
       <c r="E3">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F3" s="2">
+        <v>21.1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -515,8 +533,14 @@
       <c r="E4">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>22.9</v>
+      </c>
+      <c r="G4" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -532,8 +556,14 @@
       <c r="E5">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F5" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +579,14 @@
       <c r="E6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -566,8 +602,14 @@
       <c r="E7">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F7" s="2">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -583,8 +625,14 @@
       <c r="E8">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F8" s="2">
+        <v>21.2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,8 +648,14 @@
       <c r="E9">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F9" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="G9" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -617,8 +671,14 @@
       <c r="E10">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F10" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -634,8 +694,14 @@
       <c r="E11">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G11" s="2">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -651,8 +717,14 @@
       <c r="E12">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G12" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -668,8 +740,14 @@
       <c r="E13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F13" s="2">
+        <v>21</v>
+      </c>
+      <c r="G13" s="2">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -685,8 +763,14 @@
       <c r="E14">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F14" s="2">
+        <v>18.7</v>
+      </c>
+      <c r="G14" s="2">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -702,8 +786,14 @@
       <c r="E15">
         <v>17.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F15" s="2">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -719,8 +809,14 @@
       <c r="E16">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F16" s="2">
+        <v>23.7</v>
+      </c>
+      <c r="G16" s="2">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -736,8 +832,14 @@
       <c r="E17">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F17" s="2">
+        <v>20.7</v>
+      </c>
+      <c r="G17" s="2">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -753,8 +855,14 @@
       <c r="E18">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F18" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G18" s="2">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -770,8 +878,14 @@
       <c r="E19">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F19" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="G19" s="2">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -787,8 +901,14 @@
       <c r="E20">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F20" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -804,8 +924,14 @@
       <c r="E21">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F21" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="G21" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -821,8 +947,14 @@
       <c r="E22">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F22" s="2">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -838,8 +970,14 @@
       <c r="E23">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F23" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G23" s="2">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -855,8 +993,14 @@
       <c r="E24">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F24" s="2">
+        <v>21.4</v>
+      </c>
+      <c r="G24" s="2">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -872,8 +1016,14 @@
       <c r="E25">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F25" s="2">
+        <v>21.7</v>
+      </c>
+      <c r="G25" s="2">
+        <v>22.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -889,8 +1039,14 @@
       <c r="E26">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F26" s="2">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -905,6 +1061,12 @@
       </c>
       <c r="E27">
         <v>19.3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>21.1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications for 20 minutes pres
</commit_message>
<xml_diff>
--- a/young-DSS-exp2/new_weight_measurement.xlsx
+++ b/young-DSS-exp2/new_weight_measurement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\young-DSS-exp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C854A707-F05E-4EC9-A89F-4C92846F8601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC3690-3083-4F00-AFF7-A5FC79F1CD3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{B39F8DC0-D618-4399-8ED4-92D19BDDA9D8}"/>
   </bookViews>
@@ -440,15 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9694913F-0376-40DD-B748-937DACB00989}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E1" sqref="E1:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +470,17 @@
       <c r="G1" s="1">
         <v>45371</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H1" s="1">
+        <v>45378</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45385</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -493,8 +502,17 @@
       <c r="G2" s="2">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H2" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>20.6</v>
+      </c>
+      <c r="J2" s="2">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -516,8 +534,17 @@
       <c r="G3" s="2">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H3" s="2">
+        <v>22.3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="J3" s="2">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -539,8 +566,17 @@
       <c r="G4" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H4" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>24</v>
+      </c>
+      <c r="J4" s="2">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -562,8 +598,17 @@
       <c r="G5" s="2">
         <v>22.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H5" s="2">
+        <v>23.8</v>
+      </c>
+      <c r="I5" s="2">
+        <v>23.7</v>
+      </c>
+      <c r="J5" s="2">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -585,8 +630,17 @@
       <c r="G6" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H6" s="2">
+        <v>23.1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J6" s="2">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -608,8 +662,17 @@
       <c r="G7" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H7" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J7" s="2">
+        <v>20.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -631,8 +694,17 @@
       <c r="G8" s="2">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H8" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>21.2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -654,8 +726,17 @@
       <c r="G9" s="2">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H9" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="I9" s="2">
+        <v>21.3</v>
+      </c>
+      <c r="J9" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -677,8 +758,17 @@
       <c r="G10" s="2">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H10" s="2">
+        <v>21.1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="J10" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -700,8 +790,17 @@
       <c r="G11" s="2">
         <v>21.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H11" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="I11" s="2">
+        <v>21.7</v>
+      </c>
+      <c r="J11" s="2">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -723,8 +822,17 @@
       <c r="G12" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H12" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="J12" s="2">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -746,8 +854,17 @@
       <c r="G13" s="2">
         <v>22.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H13" s="2">
+        <v>22.2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="J13" s="2">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -769,8 +886,17 @@
       <c r="G14" s="2">
         <v>20.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H14" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="J14" s="2">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -792,8 +918,17 @@
       <c r="G15" s="2">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H15" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="I15" s="2">
+        <v>21</v>
+      </c>
+      <c r="J15" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -815,8 +950,17 @@
       <c r="G16" s="2">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H16" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="I16" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -838,8 +982,17 @@
       <c r="G17" s="2">
         <v>21.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H17" s="2">
+        <v>23.2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>22.5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -861,8 +1014,17 @@
       <c r="G18" s="2">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H18" s="2">
+        <v>22</v>
+      </c>
+      <c r="I18" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="J18" s="2">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -884,8 +1046,17 @@
       <c r="G19" s="2">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H19" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="I19" s="2">
+        <v>22</v>
+      </c>
+      <c r="J19" s="2">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -907,8 +1078,17 @@
       <c r="G20" s="2">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H20" s="2">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="J20" s="2">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -930,8 +1110,17 @@
       <c r="G21" s="2">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H21" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="I21" s="2">
+        <v>21.8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -953,8 +1142,17 @@
       <c r="G22" s="2">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H22" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>19.7</v>
+      </c>
+      <c r="J22" s="2">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
@@ -976,8 +1174,17 @@
       <c r="G23" s="2">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H23" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="I23" s="2">
+        <v>21.2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
@@ -999,8 +1206,17 @@
       <c r="G24" s="2">
         <v>23.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H24" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="I24" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="J24" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -1022,8 +1238,17 @@
       <c r="G25" s="2">
         <v>22.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H25" s="2">
+        <v>24.3</v>
+      </c>
+      <c r="I25" s="2">
+        <v>23</v>
+      </c>
+      <c r="J25" s="2">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1045,8 +1270,17 @@
       <c r="G26" s="2">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H26" s="2">
+        <v>20.6</v>
+      </c>
+      <c r="I26" s="2">
+        <v>20.7</v>
+      </c>
+      <c r="J26" s="2">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1067,6 +1301,15 @@
       </c>
       <c r="G27" s="2">
         <v>22</v>
+      </c>
+      <c r="H27" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="J27" s="2">
+        <v>23.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>